<commit_message>
Translated Miles' battle advice for chp3
</commit_message>
<xml_diff>
--- a/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
+++ b/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\デスクトップ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob Wai\Roming\サキュバス戦記new\English translation\Dreamon-Senki-Translation\English translation\その他文字 (Items, Skills, Characters, Descriptions)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F9CD555-8AE5-492A-B89F-7147DB634BA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="2172" windowWidth="11820" windowHeight="8964" xr2:uid="{A22803D4-50FF-4295-8293-4B5FFCBE5CEB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13354" windowHeight="5957"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -946,12 +945,6 @@
     <t>神秘のメダル</t>
   </si>
   <si>
-    <t>王紋の首飾り</t>
-  </si>
-  <si>
-    <t>王家の紋章が刻まれた首飾り。特殊な魔力を放つ</t>
-  </si>
-  <si>
     <t>誘惑する口穴</t>
   </si>
   <si>
@@ -1149,24 +1142,30 @@
   </si>
   <si>
     <t>精神+1、速さ+8、移動+1</t>
+  </si>
+  <si>
+    <t>A necklace engraved with the crest of the holy family.  Holds an unknown power.</t>
+  </si>
+  <si>
+    <t>King Crest Necklace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1200,7 +1199,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1511,19 +1510,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A4E8CF-D70C-4D97-8FFF-088E15A8A805}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="17.59765625" customWidth="1"/>
+    <col min="1" max="1" width="17.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1555,7 +1554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1563,7 +1562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1579,7 +1578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1587,7 +1586,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1611,7 +1610,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1619,7 +1618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1643,7 +1642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1651,7 +1650,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1659,7 +1658,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1667,7 +1666,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1683,7 +1682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1699,7 +1698,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1755,7 +1754,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1763,7 +1762,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1779,7 +1778,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1803,7 +1802,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -1811,7 +1810,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1819,7 +1818,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -1827,7 +1826,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -1835,7 +1834,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -1859,7 +1858,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>83</v>
       </c>
@@ -1883,7 +1882,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -1899,7 +1898,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>89</v>
       </c>
@@ -1907,7 +1906,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -1915,7 +1914,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -1923,7 +1922,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>97</v>
       </c>
@@ -1939,7 +1938,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>99</v>
       </c>
@@ -1947,7 +1946,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>101</v>
       </c>
@@ -1955,7 +1954,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>105</v>
       </c>
@@ -1971,7 +1970,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>107</v>
       </c>
@@ -1979,7 +1978,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>109</v>
       </c>
@@ -1987,7 +1986,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -1995,7 +1994,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>113</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>115</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>117</v>
       </c>
@@ -2019,7 +2018,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>119</v>
       </c>
@@ -2027,7 +2026,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>121</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>123</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>125</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>127</v>
       </c>
@@ -2059,7 +2058,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>129</v>
       </c>
@@ -2067,7 +2066,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>131</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>133</v>
       </c>
@@ -2083,7 +2082,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>135</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>137</v>
       </c>
@@ -2099,7 +2098,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>139</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>141</v>
       </c>
@@ -2115,7 +2114,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>143</v>
       </c>
@@ -2123,7 +2122,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>145</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>147</v>
       </c>
@@ -2139,7 +2138,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>149</v>
       </c>
@@ -2147,7 +2146,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>151</v>
       </c>
@@ -2155,7 +2154,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -2163,7 +2162,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>155</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>157</v>
       </c>
@@ -2179,7 +2178,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>159</v>
       </c>
@@ -2187,7 +2186,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>161</v>
       </c>
@@ -2195,7 +2194,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>163</v>
       </c>
@@ -2203,7 +2202,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>165</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>167</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>169</v>
       </c>
@@ -2227,7 +2226,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>171</v>
       </c>
@@ -2235,7 +2234,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>173</v>
       </c>
@@ -2243,7 +2242,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>174</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>175</v>
       </c>
@@ -2259,7 +2258,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>176</v>
       </c>
@@ -2267,7 +2266,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>177</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2">
       <c r="A95" t="s">
         <v>178</v>
       </c>
@@ -2283,7 +2282,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2">
       <c r="A96" t="s">
         <v>180</v>
       </c>
@@ -2291,7 +2290,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2">
       <c r="A97" t="s">
         <v>182</v>
       </c>
@@ -2299,7 +2298,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2">
       <c r="A98" t="s">
         <v>184</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>186</v>
       </c>
@@ -2315,7 +2314,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2">
       <c r="A100" t="s">
         <v>188</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2">
       <c r="A101" t="s">
         <v>190</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2">
       <c r="A102" t="s">
         <v>192</v>
       </c>
@@ -2339,7 +2338,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2">
       <c r="A103" t="s">
         <v>194</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:2">
       <c r="A104" t="s">
         <v>196</v>
       </c>
@@ -2355,7 +2354,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2">
       <c r="A105" t="s">
         <v>198</v>
       </c>
@@ -2363,7 +2362,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2">
       <c r="A106" t="s">
         <v>200</v>
       </c>
@@ -2371,7 +2370,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>202</v>
       </c>
@@ -2379,7 +2378,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:2">
       <c r="A108" t="s">
         <v>204</v>
       </c>
@@ -2387,7 +2386,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2">
       <c r="A109" t="s">
         <v>206</v>
       </c>
@@ -2395,7 +2394,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2">
       <c r="A110" t="s">
         <v>209</v>
       </c>
@@ -2403,7 +2402,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2">
       <c r="A111" t="s">
         <v>208</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2">
       <c r="A112" t="s">
         <v>211</v>
       </c>
@@ -2419,7 +2418,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2">
       <c r="A113" t="s">
         <v>214</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:2">
       <c r="A114" t="s">
         <v>215</v>
       </c>
@@ -2435,7 +2434,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:2">
       <c r="A115" t="s">
         <v>216</v>
       </c>
@@ -2443,7 +2442,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2">
       <c r="A116" t="s">
         <v>218</v>
       </c>
@@ -2451,7 +2450,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2">
       <c r="A117" t="s">
         <v>219</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2">
       <c r="A118" t="s">
         <v>221</v>
       </c>
@@ -2467,7 +2466,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:2">
       <c r="A119" t="s">
         <v>223</v>
       </c>
@@ -2475,7 +2474,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2">
       <c r="A120" t="s">
         <v>225</v>
       </c>
@@ -2483,7 +2482,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2">
       <c r="A121" t="s">
         <v>227</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2">
       <c r="A122" t="s">
         <v>229</v>
       </c>
@@ -2499,7 +2498,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2">
       <c r="A123" t="s">
         <v>231</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2">
       <c r="A124" t="s">
         <v>233</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2">
       <c r="A125" t="s">
         <v>235</v>
       </c>
@@ -2523,7 +2522,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2">
       <c r="A126" t="s">
         <v>237</v>
       </c>
@@ -2531,77 +2530,77 @@
         <v>238</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2">
       <c r="A127" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2">
       <c r="A128" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2">
       <c r="A129" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2">
       <c r="A130" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2">
       <c r="A131" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2">
       <c r="A132" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2">
       <c r="A133" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2">
       <c r="A135" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2">
       <c r="A136" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2">
       <c r="A137" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:2">
       <c r="A138" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2">
       <c r="A139" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2">
       <c r="A140" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2">
       <c r="A141" t="s">
         <v>253</v>
       </c>
@@ -2609,7 +2608,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2">
       <c r="A142" t="s">
         <v>255</v>
       </c>
@@ -2617,7 +2616,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2">
       <c r="A143" t="s">
         <v>257</v>
       </c>
@@ -2625,7 +2624,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2">
       <c r="A144" t="s">
         <v>259</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2">
       <c r="A145" t="s">
         <v>261</v>
       </c>
@@ -2641,7 +2640,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2">
       <c r="A146" t="s">
         <v>263</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2">
       <c r="A147" t="s">
         <v>265</v>
       </c>
@@ -2657,7 +2656,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2">
       <c r="A148" t="s">
         <v>267</v>
       </c>
@@ -2665,7 +2664,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2">
       <c r="A149" t="s">
         <v>269</v>
       </c>
@@ -2673,7 +2672,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2">
       <c r="A150" t="s">
         <v>271</v>
       </c>
@@ -2681,7 +2680,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:2">
       <c r="A151" t="s">
         <v>273</v>
       </c>
@@ -2689,7 +2688,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:2">
       <c r="A152" t="s">
         <v>275</v>
       </c>
@@ -2697,7 +2696,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2">
       <c r="A153" t="s">
         <v>277</v>
       </c>
@@ -2705,7 +2704,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:2">
       <c r="A154" t="s">
         <v>279</v>
       </c>
@@ -2713,7 +2712,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:2">
       <c r="A155" t="s">
         <v>280</v>
       </c>
@@ -2721,7 +2720,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:2">
       <c r="A156" t="s">
         <v>282</v>
       </c>
@@ -2729,7 +2728,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:2">
       <c r="A157" t="s">
         <v>284</v>
       </c>
@@ -2737,7 +2736,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:2">
       <c r="A158" t="s">
         <v>285</v>
       </c>
@@ -2745,7 +2744,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:2">
       <c r="A159" t="s">
         <v>287</v>
       </c>
@@ -2753,7 +2752,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:2">
       <c r="A160" t="s">
         <v>289</v>
       </c>
@@ -2761,7 +2760,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:2">
       <c r="A161" t="s">
         <v>291</v>
       </c>
@@ -2769,7 +2768,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:2">
       <c r="A162" t="s">
         <v>293</v>
       </c>
@@ -2777,7 +2776,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:2">
       <c r="A163" t="s">
         <v>295</v>
       </c>
@@ -2785,7 +2784,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:2">
       <c r="A164" t="s">
         <v>297</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:2">
       <c r="A165" t="s">
         <v>299</v>
       </c>
@@ -2801,7 +2800,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>301</v>
       </c>
@@ -2809,284 +2808,284 @@
         <v>300</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:2">
       <c r="A167" t="s">
+        <v>369</v>
+      </c>
+      <c r="B167" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>330</v>
+      </c>
+      <c r="B168" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
         <v>302</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B169" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A168" t="s">
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>304</v>
+      </c>
+      <c r="B170" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>306</v>
+      </c>
+      <c r="B171" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>306</v>
+      </c>
+      <c r="B172" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>309</v>
+      </c>
+      <c r="B173" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>311</v>
+      </c>
+      <c r="B174" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>311</v>
+      </c>
+      <c r="B175" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>314</v>
+      </c>
+      <c r="B176" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>316</v>
+      </c>
+      <c r="B177" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>318</v>
+      </c>
+      <c r="B178" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>320</v>
+      </c>
+      <c r="B179" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>322</v>
+      </c>
+      <c r="B180" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>324</v>
+      </c>
+      <c r="B181" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>326</v>
+      </c>
+      <c r="B182" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>328</v>
+      </c>
+      <c r="B183" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
         <v>332</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B184" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A169" t="s">
-        <v>304</v>
-      </c>
-      <c r="B169" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A170" t="s">
-        <v>306</v>
-      </c>
-      <c r="B170" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A171" t="s">
-        <v>308</v>
-      </c>
-      <c r="B171" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A172" t="s">
-        <v>308</v>
-      </c>
-      <c r="B172" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A173" t="s">
-        <v>311</v>
-      </c>
-      <c r="B173" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A174" t="s">
-        <v>313</v>
-      </c>
-      <c r="B174" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A175" t="s">
-        <v>313</v>
-      </c>
-      <c r="B175" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A176" t="s">
-        <v>316</v>
-      </c>
-      <c r="B176" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A177" t="s">
-        <v>318</v>
-      </c>
-      <c r="B177" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A178" t="s">
-        <v>320</v>
-      </c>
-      <c r="B178" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A179" t="s">
-        <v>322</v>
-      </c>
-      <c r="B179" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A180" t="s">
-        <v>324</v>
-      </c>
-      <c r="B180" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A181" t="s">
-        <v>326</v>
-      </c>
-      <c r="B181" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A182" t="s">
-        <v>328</v>
-      </c>
-      <c r="B182" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A183" t="s">
-        <v>330</v>
-      </c>
-      <c r="B183" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A184" t="s">
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
         <v>334</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B185" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A185" t="s">
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
         <v>336</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B186" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A186" t="s">
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
         <v>338</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B187" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A187" t="s">
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
         <v>340</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B188" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A188" t="s">
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
         <v>342</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B189" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A189" t="s">
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
         <v>344</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B190" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A190" t="s">
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
         <v>346</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B191" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A191" t="s">
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
         <v>348</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B192" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A192" t="s">
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
         <v>350</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B193" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A193" t="s">
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
         <v>352</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B194" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A194" t="s">
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
         <v>354</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B195" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A195" t="s">
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
         <v>356</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B196" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A196" t="s">
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
         <v>358</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B197" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A197" t="s">
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
         <v>360</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B198" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A198" t="s">
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
         <v>362</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B199" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A199" t="s">
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
         <v>364</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B200" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A200" t="s">
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
         <v>366</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B201" t="s">
         <v>367</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A201" t="s">
-        <v>368</v>
-      </c>
-      <c r="B201" t="s">
-        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Chapter 3 proofreading"
This reverts commit 078743557df5d57fe763db80503db3a61ff6e23b.
</commit_message>
<xml_diff>
--- a/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
+++ b/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob Wai\Roming\サキュバス戦記new\English translation\Dreamon-Senki-Translation\English translation\その他文字 (Items, Skills, Characters, Descriptions)\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13350" windowHeight="5955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13354" windowHeight="5957"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -1148,7 +1153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -1188,10 +1193,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1255,7 +1257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1307,7 +1309,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1501,7 +1503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1509,15 +1511,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I201"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.61328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2758,7 +2760,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:2">
       <c r="A161" t="s">
         <v>291</v>
       </c>
@@ -2766,7 +2768,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:2">
       <c r="A162" t="s">
         <v>293</v>
       </c>
@@ -2774,7 +2776,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:2">
       <c r="A163" t="s">
         <v>295</v>
       </c>
@@ -2782,7 +2784,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:2">
       <c r="A164" t="s">
         <v>297</v>
       </c>
@@ -2790,7 +2792,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:2">
       <c r="A165" t="s">
         <v>299</v>
       </c>
@@ -2798,7 +2800,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>301</v>
       </c>
@@ -2806,22 +2808,15 @@
         <v>300</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:2">
       <c r="A167" t="s">
         <v>369</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" t="s">
         <v>368</v>
       </c>
-      <c r="C167" s="1"/>
-      <c r="D167" s="1"/>
-      <c r="E167" s="1"/>
-      <c r="F167" s="1"/>
-      <c r="G167" s="1"/>
-      <c r="H167" s="1"/>
-      <c r="I167" s="1"/>
-    </row>
-    <row r="168" spans="1:9">
+    </row>
+    <row r="168" spans="1:2">
       <c r="A168" t="s">
         <v>330</v>
       </c>
@@ -2829,7 +2824,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:2">
       <c r="A169" t="s">
         <v>302</v>
       </c>
@@ -2837,7 +2832,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="170" spans="1:9">
+    <row r="170" spans="1:2">
       <c r="A170" t="s">
         <v>304</v>
       </c>
@@ -2845,7 +2840,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:2">
       <c r="A171" t="s">
         <v>306</v>
       </c>
@@ -2853,7 +2848,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:2">
       <c r="A172" t="s">
         <v>306</v>
       </c>
@@ -2861,7 +2856,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:2">
       <c r="A173" t="s">
         <v>309</v>
       </c>
@@ -2869,7 +2864,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:2">
       <c r="A174" t="s">
         <v>311</v>
       </c>
@@ -2877,7 +2872,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:2">
       <c r="A175" t="s">
         <v>311</v>
       </c>
@@ -2885,7 +2880,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>314</v>
       </c>
@@ -3094,9 +3089,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B167:I167"/>
-  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Revert "Chapter 3 proofreading""
This reverts commit b15e9fcaeb6f92d29f035dc1043a08b4ed5abf3c.
</commit_message>
<xml_diff>
--- a/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
+++ b/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob Wai\Roming\サキュバス戦記new\English translation\Dreamon-Senki-Translation\English translation\その他文字 (Items, Skills, Characters, Descriptions)\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13354" windowHeight="5957"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13350" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -1153,7 +1148,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -1193,7 +1188,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1257,7 +1255,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1309,7 +1307,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1503,7 +1501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1511,15 +1509,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:I201"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="C174" sqref="C174"/>
+      <selection activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.61328125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2760,7 +2758,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:9">
       <c r="A161" t="s">
         <v>291</v>
       </c>
@@ -2768,7 +2766,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:9">
       <c r="A162" t="s">
         <v>293</v>
       </c>
@@ -2776,7 +2774,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:9">
       <c r="A163" t="s">
         <v>295</v>
       </c>
@@ -2784,7 +2782,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:9">
       <c r="A164" t="s">
         <v>297</v>
       </c>
@@ -2792,7 +2790,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:9">
       <c r="A165" t="s">
         <v>299</v>
       </c>
@@ -2800,7 +2798,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:9">
       <c r="A166" t="s">
         <v>301</v>
       </c>
@@ -2808,15 +2806,22 @@
         <v>300</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:9">
       <c r="A167" t="s">
         <v>369</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="1" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="168" spans="1:2">
+      <c r="C167" s="1"/>
+      <c r="D167" s="1"/>
+      <c r="E167" s="1"/>
+      <c r="F167" s="1"/>
+      <c r="G167" s="1"/>
+      <c r="H167" s="1"/>
+      <c r="I167" s="1"/>
+    </row>
+    <row r="168" spans="1:9">
       <c r="A168" t="s">
         <v>330</v>
       </c>
@@ -2824,7 +2829,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:9">
       <c r="A169" t="s">
         <v>302</v>
       </c>
@@ -2832,7 +2837,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:9">
       <c r="A170" t="s">
         <v>304</v>
       </c>
@@ -2840,7 +2845,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:9">
       <c r="A171" t="s">
         <v>306</v>
       </c>
@@ -2848,7 +2853,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:9">
       <c r="A172" t="s">
         <v>306</v>
       </c>
@@ -2856,7 +2861,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:9">
       <c r="A173" t="s">
         <v>309</v>
       </c>
@@ -2864,7 +2869,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:9">
       <c r="A174" t="s">
         <v>311</v>
       </c>
@@ -2872,7 +2877,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:9">
       <c r="A175" t="s">
         <v>311</v>
       </c>
@@ -2880,7 +2885,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:9">
       <c r="A176" t="s">
         <v>314</v>
       </c>
@@ -3089,6 +3094,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B167:I167"/>
+  </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Items and weapons translation
</commit_message>
<xml_diff>
--- a/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
+++ b/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
@@ -1513,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="D141" sqref="D141"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>

</xml_diff>

<commit_message>
Items and weapon updates (Changed main hero relic names)
</commit_message>
<xml_diff>
--- a/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
+++ b/English translation/その他文字 (Items, Skills, Characters, Descriptions)/items.xlsx
@@ -29,225 +29,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="370">
-  <si>
-    <t>封呪の布</t>
-  </si>
-  <si>
-    <t>呪いを抑える力のある布。元は聖剣に巻いてあった。腕に巻き付けて包帯のように使う。</t>
-  </si>
-  <si>
-    <t>女性キャラ雇用権</t>
-  </si>
-  <si>
-    <t>クリアしたステージの敵淫魔を酒場で仲間にできます。</t>
-  </si>
-  <si>
-    <t>力減少薬</t>
-  </si>
-  <si>
-    <t>相手の「力」を永続的に-1する。</t>
-  </si>
-  <si>
-    <t>守備減少薬</t>
-  </si>
-  <si>
-    <t>相手の「守備力」を永続的に-1する。</t>
-  </si>
-  <si>
-    <t>魔力減少薬</t>
-  </si>
-  <si>
-    <t>相手の「魔力」を永続的に-1する。</t>
-  </si>
-  <si>
-    <t>技減少薬</t>
-  </si>
-  <si>
-    <t>速さ減少薬</t>
-  </si>
-  <si>
-    <t>相手の「速さ」を永続的に-1する。</t>
-  </si>
-  <si>
-    <t>全能力減少薬</t>
-  </si>
-  <si>
-    <t>相手の全能力を永続的に-2する。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ニガムシの葉</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="371">
   <si>
     <t>ちぎってなめると苦みから正気に戻る葉。魅了・発情から回復する。</t>
   </si>
   <si>
-    <t>風のマント</t>
-  </si>
-  <si>
     <t>エルフからもらったマント。所持していると速さ+5。</t>
   </si>
   <si>
-    <t>俊足ブーツ</t>
-  </si>
-  <si>
     <t>所持していると移動力が１上がる。</t>
   </si>
   <si>
-    <t>韋駄天の靴</t>
-  </si>
-  <si>
     <t>所持していると移動力が3上がる。</t>
   </si>
   <si>
-    <t>超俊足ブーツ</t>
-  </si>
-  <si>
     <t>所持していると移動力が12上がる。</t>
   </si>
   <si>
-    <t>超成長の珠</t>
-  </si>
-  <si>
     <t>所持しているとレベルアップ時に成長補正がかかる宝玉。</t>
   </si>
   <si>
-    <t>癒しの宝玉</t>
-  </si>
-  <si>
     <t>自身の体力を25回復する（何回でも使用可能）</t>
   </si>
   <si>
-    <t>生命の宝玉</t>
-  </si>
-  <si>
     <t>所持していると毎ターン10自然回復する。</t>
   </si>
   <si>
-    <t>時戻しの宝玉</t>
-  </si>
-  <si>
     <t>時空をゆがめて味方全体をもう一度行動可能にする宝玉。一度しか使えない。</t>
   </si>
   <si>
-    <t>鉄アレイ</t>
-  </si>
-  <si>
     <t>所持していると力が少し伸びやすくなる。</t>
   </si>
   <si>
-    <t>スタミナスーツ</t>
-  </si>
-  <si>
     <t>重りを入れた服。所持しているとHPが少し伸びやすくなる。</t>
   </si>
   <si>
-    <t>重り入りブーツ</t>
-  </si>
-  <si>
     <t>所持していると速さが少し伸びやすくなる。</t>
   </si>
   <si>
-    <t>器用グローブ</t>
-  </si>
-  <si>
     <t>所持していると技が少し伸びやすくなる。</t>
   </si>
   <si>
-    <t>神秘のコケ</t>
-  </si>
-  <si>
     <t>所持していると魔力が少し伸びやすくなる。</t>
   </si>
   <si>
-    <t>元気フラッグ</t>
-  </si>
-  <si>
     <t>所持しているとHPの成長にやや大きなボーナスが付く。</t>
   </si>
   <si>
-    <t>おもちゃの人形</t>
-  </si>
-  <si>
     <t>少年がくれたおもちゃの人形。所持していると心を強く持てる。</t>
   </si>
   <si>
-    <t>エルフのお守り</t>
-  </si>
-  <si>
     <t>精神力+1、魔力+2、幸運+2</t>
   </si>
   <si>
-    <t>四葉のクローバー</t>
-  </si>
-  <si>
     <t>幸運+10</t>
   </si>
   <si>
-    <t>ヘビーアーマー</t>
-  </si>
-  <si>
     <t>重い鎧で防御力抜群。</t>
   </si>
   <si>
-    <t>スモールシールド</t>
-  </si>
-  <si>
     <t>小さな金属製の盾</t>
   </si>
   <si>
-    <t>クラスチェンジの証</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>所持しているとクラスチェンジができるようになる。</t>
   </si>
   <si>
-    <t>ヒールの魔術書</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>味方一人の体力を25回復する(射程全域)。</t>
   </si>
   <si>
-    <t>癒しの杖</t>
-  </si>
-  <si>
     <t>味方一人の体力を30回復する杖。射程２。</t>
   </si>
   <si>
-    <t>大回復の杖</t>
-  </si>
-  <si>
     <t>味方一人の体力を60回復する杖。射程２。</t>
   </si>
   <si>
-    <t>大森林の杖</t>
-  </si>
-  <si>
     <t>味方一人の体力を30回復する杖。素材の木がよく、魔力が遠くまで届く。</t>
   </si>
   <si>
-    <t>全体回復の杖（弱）</t>
-  </si>
-  <si>
     <t>味方全員の体力を8回復する杖。</t>
   </si>
   <si>
-    <t>全体回復の杖（中）</t>
-  </si>
-  <si>
     <t>味方全員の体力を25回復する杖。</t>
   </si>
   <si>
-    <t>全体回復の杖（大）</t>
-  </si>
-  <si>
     <t>味方全員の体力を65回復する杖。</t>
-  </si>
-  <si>
-    <t>祈りの杖</t>
   </si>
   <si>
     <t>範囲6の味方の体力を魔力分だけ回復する杖。耐久に優れる。</t>
@@ -377,9 +242,6 @@
     <t>ふつうの兵士。</t>
   </si>
   <si>
-    <t>エリート雑兵</t>
-  </si>
-  <si>
     <t>才能のある兵士。</t>
   </si>
   <si>
@@ -390,19 +252,10 @@
     <t>味方の基礎ステを上げられる。戦闘力は低い</t>
   </si>
   <si>
-    <t>発掘家</t>
-  </si>
-  <si>
     <t>特技「発掘」でアイテムを収集できる</t>
   </si>
   <si>
-    <t>ランサー</t>
-  </si>
-  <si>
     <t>「技」の高い槍使い</t>
-  </si>
-  <si>
-    <t>ヒーラー</t>
   </si>
   <si>
     <t>回復の杖が使える癒し手</t>
@@ -1144,10 +997,157 @@
     <t>Increases resistance by 2 when held.</t>
   </si>
   <si>
-    <t>Kazemaken</t>
-  </si>
-  <si>
-    <t>Hikarimaken</t>
+    <t>Permantly decreases foe's defence by 1 after combat.</t>
+  </si>
+  <si>
+    <t>Strength Sap</t>
+  </si>
+  <si>
+    <t>Defense Sap</t>
+  </si>
+  <si>
+    <t>Magic Sap</t>
+  </si>
+  <si>
+    <t>Skill Sap</t>
+  </si>
+  <si>
+    <t>Speed Sap</t>
+  </si>
+  <si>
+    <t>Vaunted Sap</t>
+  </si>
+  <si>
+    <t>Permantly decreases foe's strength by 1 after combat.</t>
+  </si>
+  <si>
+    <t>Permantly decreases foe's skill by 1 after combat.</t>
+  </si>
+  <si>
+    <t>Permantly decreases foe's magic by 1 after combat.</t>
+  </si>
+  <si>
+    <t>Permantly decreases foe's speed by 1 after combat.</t>
+  </si>
+  <si>
+    <t>Permantly decreases all foe's stats by 2 after combat.</t>
+  </si>
+  <si>
+    <t>Female Recruitment Deploma</t>
+  </si>
+  <si>
+    <t>When held, allows female succubus enemies from past chapters to be recruited.</t>
+  </si>
+  <si>
+    <t>Amihan</t>
+  </si>
+  <si>
+    <t>Mithrus</t>
+  </si>
+  <si>
+    <t>Sealed Cloth Sigil</t>
+  </si>
+  <si>
+    <t>A cloth with the power to surpress curses. Originaly wrapped around the holy sword Mithrus. It's used to cover the hilt of the sword.</t>
+  </si>
+  <si>
+    <t>Sour Leaf</t>
+  </si>
+  <si>
+    <t>Swift Mantle</t>
+  </si>
+  <si>
+    <t>Pegasus Boots</t>
+  </si>
+  <si>
+    <t>Dash Boots</t>
+  </si>
+  <si>
+    <t>Boots of Hermes</t>
+  </si>
+  <si>
+    <t>Ultra Growth Gem</t>
+  </si>
+  <si>
+    <t>Gem of Healing</t>
+  </si>
+  <si>
+    <t>Gem of Life</t>
+  </si>
+  <si>
+    <t>Turnwheel Gem</t>
+  </si>
+  <si>
+    <t>Iron Dumbbells</t>
+  </si>
+  <si>
+    <t>Stamina Suit</t>
+  </si>
+  <si>
+    <t>Weighted Boots</t>
+  </si>
+  <si>
+    <t>Dexterous glove</t>
+  </si>
+  <si>
+    <t>Mystery Moss</t>
+  </si>
+  <si>
+    <t>Lively Flag</t>
+  </si>
+  <si>
+    <t>Toy Doll</t>
+  </si>
+  <si>
+    <t>Elf's Amulet</t>
+  </si>
+  <si>
+    <t>Fourleafed Clover</t>
+  </si>
+  <si>
+    <t>Heavy Armour</t>
+  </si>
+  <si>
+    <t>Small Shield</t>
+  </si>
+  <si>
+    <t>Class Change Certificate</t>
+  </si>
+  <si>
+    <t>Healing Tome</t>
+  </si>
+  <si>
+    <t>Healing Cane</t>
+  </si>
+  <si>
+    <t>Healing Staff</t>
+  </si>
+  <si>
+    <t>Forest Staff</t>
+  </si>
+  <si>
+    <t>All Recovery Staff (Weak)</t>
+  </si>
+  <si>
+    <t>All Recovery Staff (Medium)</t>
+  </si>
+  <si>
+    <t>All Recovery Staff (Strong)</t>
+  </si>
+  <si>
+    <t>Prayer Staff</t>
+  </si>
+  <si>
+    <t>Lancer</t>
+  </si>
+  <si>
+    <t>Healer</t>
+  </si>
+  <si>
+    <t>Discoverable House</t>
+  </si>
+  <si>
+    <t>Elite Soilder</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1514,7 @@
   <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -1524,1568 +1524,1568 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>368</v>
+        <v>334</v>
       </c>
       <c r="B1" t="s">
-        <v>307</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s">
-        <v>306</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>336</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>332</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="B6" t="s">
-        <v>295</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="B7" t="s">
-        <v>296</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>298</v>
+        <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="B9" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
       <c r="B10" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>302</v>
+        <v>254</v>
       </c>
       <c r="B11" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
       <c r="B12" t="s">
-        <v>311</v>
+        <v>263</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>316</v>
+        <v>268</v>
       </c>
       <c r="B13" t="s">
-        <v>312</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>304</v>
+        <v>256</v>
       </c>
       <c r="B14" t="s">
-        <v>313</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>305</v>
+        <v>257</v>
       </c>
       <c r="B15" t="s">
-        <v>314</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>308</v>
+        <v>260</v>
       </c>
       <c r="B16" t="s">
-        <v>309</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>303</v>
+        <v>255</v>
       </c>
       <c r="B17" t="s">
-        <v>315</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>269</v>
       </c>
       <c r="B18" t="s">
-        <v>319</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>318</v>
+        <v>270</v>
       </c>
       <c r="B19" t="s">
-        <v>320</v>
+        <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>324</v>
+        <v>276</v>
       </c>
       <c r="B20" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="B21" t="s">
-        <v>322</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="B22" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="B23" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="B24" t="s">
-        <v>331</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>330</v>
+        <v>282</v>
       </c>
       <c r="B25" t="s">
-        <v>332</v>
+        <v>284</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>321</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>322</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>323</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>324</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>325</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>326</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>331</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>333</v>
+        <v>285</v>
       </c>
       <c r="B32" t="s">
-        <v>335</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="B33" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>337</v>
+        <v>289</v>
       </c>
       <c r="B34" t="s">
-        <v>338</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>339</v>
+        <v>291</v>
       </c>
       <c r="B35" t="s">
-        <v>340</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>341</v>
+        <v>293</v>
       </c>
       <c r="B36" t="s">
-        <v>342</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="B37" t="s">
-        <v>344</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="B38" t="s">
-        <v>348</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>346</v>
+        <v>298</v>
       </c>
       <c r="B39" t="s">
-        <v>347</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>349</v>
+        <v>301</v>
       </c>
       <c r="B40" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>351</v>
+        <v>303</v>
       </c>
       <c r="B41" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="B42" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>355</v>
+        <v>307</v>
       </c>
       <c r="B43" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="B44" t="s">
-        <v>358</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>357</v>
+        <v>309</v>
       </c>
       <c r="B45" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>359</v>
+        <v>311</v>
       </c>
       <c r="B46" t="s">
-        <v>360</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>338</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>339</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>341</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>340</v>
       </c>
       <c r="B50" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>342</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>343</v>
       </c>
       <c r="B52" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>344</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>29</v>
+        <v>345</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>346</v>
       </c>
       <c r="B55" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>347</v>
       </c>
       <c r="B56" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>348</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>349</v>
       </c>
       <c r="B58" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>39</v>
+        <v>350</v>
       </c>
       <c r="B59" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>41</v>
+        <v>351</v>
       </c>
       <c r="B60" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>352</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>353</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>47</v>
+        <v>354</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>49</v>
+        <v>355</v>
       </c>
       <c r="B64" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>356</v>
       </c>
       <c r="B65" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>53</v>
+        <v>357</v>
       </c>
       <c r="B66" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>55</v>
+        <v>358</v>
       </c>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>57</v>
+        <v>359</v>
       </c>
       <c r="B68" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>59</v>
+        <v>360</v>
       </c>
       <c r="B69" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>361</v>
       </c>
       <c r="B70" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>362</v>
       </c>
       <c r="B71" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>363</v>
       </c>
       <c r="B72" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>364</v>
       </c>
       <c r="B73" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>365</v>
       </c>
       <c r="B74" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>366</v>
       </c>
       <c r="B75" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="B78" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="B80" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="B83" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="B84" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="B85" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="B86" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="B87" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="B88" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="B89" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="B93" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="B94" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B96" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="B97" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="B98" t="s">
-        <v>113</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>114</v>
+        <v>370</v>
       </c>
       <c r="B99" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="B100" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>118</v>
+        <v>369</v>
       </c>
       <c r="B101" t="s">
-        <v>119</v>
+        <v>73</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>120</v>
+        <v>367</v>
       </c>
       <c r="B102" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>122</v>
+        <v>368</v>
       </c>
       <c r="B103" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="B104" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="B105" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
       <c r="B106" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="B108" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="B109" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="B110" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="B111" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>139</v>
+        <v>91</v>
       </c>
       <c r="B112" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="B113" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="B114" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="B115" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="B116" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="B117" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
       <c r="B118" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="B119" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="B120" t="s">
-        <v>154</v>
+        <v>106</v>
       </c>
     </row>
     <row r="121" spans="1:2">
       <c r="A121" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="B121" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="B122" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="B123" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
       <c r="B124" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="B125" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>165</v>
+        <v>117</v>
       </c>
       <c r="B126" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>278</v>
+        <v>230</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>279</v>
+        <v>231</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>280</v>
+        <v>232</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>281</v>
+        <v>233</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>282</v>
+        <v>234</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>283</v>
+        <v>235</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>284</v>
+        <v>236</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>286</v>
+        <v>238</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>287</v>
+        <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>288</v>
+        <v>240</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>289</v>
+        <v>241</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>290</v>
+        <v>242</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>363</v>
+        <v>315</v>
       </c>
       <c r="B141" t="s">
-        <v>362</v>
+        <v>314</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>364</v>
+        <v>316</v>
       </c>
       <c r="B142" t="s">
-        <v>366</v>
+        <v>318</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>365</v>
+        <v>317</v>
       </c>
       <c r="B143" t="s">
-        <v>367</v>
+        <v>319</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="B144" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="B145" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="B146" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
       <c r="B147" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
       <c r="B148" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="B149" t="s">
-        <v>178</v>
+        <v>130</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="B150" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="B151" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
       <c r="B152" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="B153" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>187</v>
+        <v>139</v>
       </c>
       <c r="B154" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>276</v>
+        <v>228</v>
       </c>
       <c r="B155" t="s">
-        <v>277</v>
+        <v>229</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="B156" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>190</v>
+        <v>142</v>
       </c>
       <c r="B157" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
       <c r="B158" t="s">
-        <v>192</v>
+        <v>144</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
       <c r="B159" t="s">
-        <v>194</v>
+        <v>146</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="B160" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>197</v>
+        <v>149</v>
       </c>
       <c r="B161" t="s">
-        <v>198</v>
+        <v>150</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>199</v>
+        <v>151</v>
       </c>
       <c r="B162" t="s">
-        <v>200</v>
+        <v>152</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="B163" t="s">
-        <v>202</v>
+        <v>154</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>203</v>
+        <v>155</v>
       </c>
       <c r="B164" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
       <c r="B165" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>207</v>
+        <v>159</v>
       </c>
       <c r="B166" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>275</v>
+        <v>227</v>
       </c>
       <c r="B167" t="s">
-        <v>274</v>
+        <v>226</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>236</v>
+        <v>188</v>
       </c>
       <c r="B168" t="s">
-        <v>237</v>
+        <v>189</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>208</v>
+        <v>160</v>
       </c>
       <c r="B169" t="s">
-        <v>209</v>
+        <v>161</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>210</v>
+        <v>162</v>
       </c>
       <c r="B170" t="s">
-        <v>211</v>
+        <v>163</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>212</v>
+        <v>164</v>
       </c>
       <c r="B171" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>212</v>
+        <v>164</v>
       </c>
       <c r="B172" t="s">
-        <v>214</v>
+        <v>166</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>215</v>
+        <v>167</v>
       </c>
       <c r="B173" t="s">
-        <v>216</v>
+        <v>168</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
       <c r="B174" t="s">
-        <v>218</v>
+        <v>170</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
       <c r="B175" t="s">
-        <v>219</v>
+        <v>171</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>220</v>
+        <v>172</v>
       </c>
       <c r="B176" t="s">
-        <v>221</v>
+        <v>173</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>222</v>
+        <v>174</v>
       </c>
       <c r="B177" t="s">
-        <v>223</v>
+        <v>175</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>225</v>
+        <v>177</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
       <c r="B180" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>230</v>
+        <v>182</v>
       </c>
       <c r="B181" t="s">
-        <v>231</v>
+        <v>183</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
       <c r="B182" t="s">
-        <v>233</v>
+        <v>185</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="B183" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>238</v>
+        <v>190</v>
       </c>
       <c r="B184" t="s">
-        <v>239</v>
+        <v>191</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="B185" t="s">
-        <v>241</v>
+        <v>193</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>242</v>
+        <v>194</v>
       </c>
       <c r="B186" t="s">
-        <v>243</v>
+        <v>195</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="B187" t="s">
-        <v>245</v>
+        <v>197</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>246</v>
+        <v>198</v>
       </c>
       <c r="B188" t="s">
-        <v>247</v>
+        <v>199</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>248</v>
+        <v>200</v>
       </c>
       <c r="B189" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>250</v>
+        <v>202</v>
       </c>
       <c r="B190" t="s">
-        <v>251</v>
+        <v>203</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>252</v>
+        <v>204</v>
       </c>
       <c r="B191" t="s">
-        <v>253</v>
+        <v>205</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>254</v>
+        <v>206</v>
       </c>
       <c r="B192" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="B193" t="s">
-        <v>257</v>
+        <v>209</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>258</v>
+        <v>210</v>
       </c>
       <c r="B194" t="s">
-        <v>259</v>
+        <v>211</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>260</v>
+        <v>212</v>
       </c>
       <c r="B195" t="s">
-        <v>261</v>
+        <v>213</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>262</v>
+        <v>214</v>
       </c>
       <c r="B196" t="s">
-        <v>263</v>
+        <v>215</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>264</v>
+        <v>216</v>
       </c>
       <c r="B197" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>266</v>
+        <v>218</v>
       </c>
       <c r="B198" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>268</v>
+        <v>220</v>
       </c>
       <c r="B199" t="s">
-        <v>269</v>
+        <v>221</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>270</v>
+        <v>222</v>
       </c>
       <c r="B200" t="s">
-        <v>271</v>
+        <v>223</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>272</v>
+        <v>224</v>
       </c>
       <c r="B201" t="s">
-        <v>273</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>